<commit_message>
-added a person.Testing Github logs.
</commit_message>
<xml_diff>
--- a/data/excel/japanese-people-data.xlsx
+++ b/data/excel/japanese-people-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">人名/本名</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t xml:space="preserve">1929年3月22日</t>
+  </si>
+  <si>
+    <t xml:space="preserve">非公開</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1995年3月6日</t>
   </si>
 </sst>
 </file>
@@ -243,7 +249,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -389,9 +395,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>

</xml_diff>